<commit_message>
i hit a wall around 15 hours of programming each day. proud of meeee. am currently working on loading composite milestones from excel. they are written correctly, but the loading replaces component milestones w an id instead of producing the json structure i expect.
</commit_message>
<xml_diff>
--- a/out/Forecast_041459.xlsx
+++ b/out/Forecast_041459.xlsx
@@ -15,18 +15,13 @@
     <sheet name="AccountMilestones" sheetId="6" r:id="rId6"/>
     <sheet name="MemoMilestones" sheetId="7" r:id="rId7"/>
     <sheet name="CompositeMilestones" sheetId="8" r:id="rId8"/>
-    <sheet name="Forecast" sheetId="9" r:id="rId9"/>
-    <sheet name="Skipped" sheetId="10" r:id="rId10"/>
-    <sheet name="Confirmed" sheetId="11" r:id="rId11"/>
-    <sheet name="Deferred" sheetId="12" r:id="rId12"/>
-    <sheet name="Milestone Results" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t>Field</t>
   </si>
@@ -58,12 +53,6 @@
     <t>041459</t>
   </si>
   <si>
-    <t>2024_02_01__02_02_24</t>
-  </si>
-  <si>
-    <t>2024_02_01__02_02_50</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -239,45 +228,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Marginal Interest</t>
-  </si>
-  <si>
-    <t>Net Gain</t>
-  </si>
-  <si>
-    <t>Net Loss</t>
-  </si>
-  <si>
-    <t>Net Worth</t>
-  </si>
-  <si>
-    <t>Loan Total</t>
-  </si>
-  <si>
-    <t>CC Debt Total</t>
-  </si>
-  <si>
-    <t>Liquid Total</t>
-  </si>
-  <si>
-    <t>p1 daily txn 1/2/00 (Checking -$100.0);  loan min payment (test loan: Principal Balance -$50.0);  cc interest (Checking -$0.08); cc min payment (Credit: Prev Stmt Bal -$39.92);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p2 daily txn 1/3/00 (Checking -$100.0); </t>
-  </si>
-  <si>
-    <t xml:space="preserve">p3 daily txn 1/4/00 (Checking -$100.0); </t>
-  </si>
-  <si>
-    <t>Result_Date</t>
-  </si>
-  <si>
-    <t>Composite</t>
   </si>
 </sst>
 </file>
@@ -642,7 +592,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -681,294 +631,10 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="nan" customWidth="1"/>
-    <col min="2" max="2" width="nan" customWidth="1"/>
-    <col min="3" max="3" width="nan" customWidth="1"/>
-    <col min="4" max="4" width="nan" customWidth="1"/>
-    <col min="5" max="5" width="nan" customWidth="1"/>
-    <col min="6" max="6" width="nan" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="nan" customWidth="1"/>
-    <col min="2" max="2" width="nan" customWidth="1"/>
-    <col min="3" max="3" width="nan" customWidth="1"/>
-    <col min="4" max="4" width="nan" customWidth="1"/>
-    <col min="5" max="5" width="nan" customWidth="1"/>
-    <col min="6" max="6" width="nan" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -999,42 +665,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>2000</v>
@@ -1046,7 +712,7 @@
         <v>100000</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -1054,7 +720,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -1066,7 +732,7 @@
         <v>20000</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -1074,7 +740,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1086,19 +752,19 @@
         <v>20000</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>0.01</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J4">
         <v>40</v>
@@ -1109,7 +775,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -1121,19 +787,19 @@
         <v>9999</v>
       </c>
       <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>35</v>
       </c>
       <c r="H5">
         <v>0.01</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J5">
         <v>50</v>
@@ -1144,7 +810,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1156,7 +822,7 @@
         <v>9999</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -1187,48 +853,48 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -1239,22 +905,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -1265,22 +931,22 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -1291,22 +957,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -1336,27 +1002,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1364,13 +1030,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1378,13 +1044,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1423,24 +1089,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
       </c>
       <c r="C2">
         <v>160</v>
@@ -1451,10 +1117,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1482,26 +1148,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1524,344 +1190,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
-    <col min="14" max="14" width="176.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2000</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1700</v>
-      </c>
-      <c r="K2">
-        <v>100</v>
-      </c>
-      <c r="L2">
-        <v>200</v>
-      </c>
-      <c r="M2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>1810</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>160.08</v>
-      </c>
-      <c r="E3">
-        <v>50</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.08</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>100.08</v>
-      </c>
-      <c r="J3">
-        <v>1599.92</v>
-      </c>
-      <c r="K3">
-        <v>50</v>
-      </c>
-      <c r="L3">
-        <v>160.08</v>
-      </c>
-      <c r="M3">
-        <v>1810</v>
-      </c>
-      <c r="N3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4">
-        <v>1710</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>160.08</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="J4">
-        <v>1499.92</v>
-      </c>
-      <c r="K4">
-        <v>50</v>
-      </c>
-      <c r="L4">
-        <v>160.08</v>
-      </c>
-      <c r="M4">
-        <v>1710</v>
-      </c>
-      <c r="N4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5">
-        <v>1610</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>160.08</v>
-      </c>
-      <c r="E5">
-        <v>50</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-      <c r="J5">
-        <v>1399.92</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
-      </c>
-      <c r="L5">
-        <v>160.08</v>
-      </c>
-      <c r="M5">
-        <v>1610</v>
-      </c>
-      <c r="N5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1610</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>160.08</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1399.92</v>
-      </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
-      <c r="L6">
-        <v>160.08</v>
-      </c>
-      <c r="M6">
-        <v>1610</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
traceback now displays front and center when a new run is submitted :)
</commit_message>
<xml_diff>
--- a/out/Forecast_041459.xlsx
+++ b/out/Forecast_041459.xlsx
@@ -15,13 +15,18 @@
     <sheet name="AccountMilestones" sheetId="6" r:id="rId6"/>
     <sheet name="MemoMilestones" sheetId="7" r:id="rId7"/>
     <sheet name="CompositeMilestones" sheetId="8" r:id="rId8"/>
+    <sheet name="Forecast" sheetId="9" r:id="rId9"/>
+    <sheet name="Skipped" sheetId="10" r:id="rId10"/>
+    <sheet name="Confirmed" sheetId="11" r:id="rId11"/>
+    <sheet name="Deferred" sheetId="12" r:id="rId12"/>
+    <sheet name="Milestone Results" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="84">
   <si>
     <t>Field</t>
   </si>
@@ -53,6 +58,12 @@
     <t>041459</t>
   </si>
   <si>
+    <t>2024_02_01__15_53_24</t>
+  </si>
+  <si>
+    <t>2024_02_01__15_53_54</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -228,6 +239,45 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Marginal Interest</t>
+  </si>
+  <si>
+    <t>Net Gain</t>
+  </si>
+  <si>
+    <t>Net Loss</t>
+  </si>
+  <si>
+    <t>Net Worth</t>
+  </si>
+  <si>
+    <t>Loan Total</t>
+  </si>
+  <si>
+    <t>CC Debt Total</t>
+  </si>
+  <si>
+    <t>Liquid Total</t>
+  </si>
+  <si>
+    <t>p1 daily txn 1/2/00 (Checking -$100.0);  loan min payment (test loan: Principal Balance -$50.0);  cc interest (Checking -$0.08); cc min payment (Credit: Prev Stmt Bal -$39.92);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p2 daily txn 1/3/00 (Checking -$100.0); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">p3 daily txn 1/4/00 (Checking -$100.0); </t>
+  </si>
+  <si>
+    <t>Result_Date</t>
+  </si>
+  <si>
+    <t>Composite</t>
   </si>
 </sst>
 </file>
@@ -592,7 +642,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -631,10 +681,294 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="nan" customWidth="1"/>
+    <col min="2" max="2" width="nan" customWidth="1"/>
+    <col min="3" max="3" width="nan" customWidth="1"/>
+    <col min="4" max="4" width="nan" customWidth="1"/>
+    <col min="5" max="5" width="nan" customWidth="1"/>
+    <col min="6" max="6" width="nan" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="nan" customWidth="1"/>
+    <col min="2" max="2" width="nan" customWidth="1"/>
+    <col min="3" max="3" width="nan" customWidth="1"/>
+    <col min="4" max="4" width="nan" customWidth="1"/>
+    <col min="5" max="5" width="nan" customWidth="1"/>
+    <col min="6" max="6" width="nan" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -665,42 +999,42 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>2000</v>
@@ -712,7 +1046,7 @@
         <v>100000</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -720,7 +1054,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -732,7 +1066,7 @@
         <v>20000</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" t="b">
         <v>0</v>
@@ -740,7 +1074,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -752,19 +1086,19 @@
         <v>20000</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>0.01</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J4">
         <v>40</v>
@@ -775,7 +1109,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -787,19 +1121,19 @@
         <v>9999</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H5">
         <v>0.01</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>50</v>
@@ -810,7 +1144,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -822,7 +1156,7 @@
         <v>9999</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
@@ -853,48 +1187,48 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -905,22 +1239,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -931,22 +1265,22 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -957,22 +1291,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -1002,27 +1336,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1030,13 +1364,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1044,13 +1378,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1089,24 +1423,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>160</v>
@@ -1117,10 +1451,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1148,26 +1482,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1190,57 +1524,344 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="176.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1700</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>200</v>
+      </c>
+      <c r="M2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>1810</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>160.08</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.08</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>100.08</v>
+      </c>
+      <c r="J3">
+        <v>1599.92</v>
+      </c>
+      <c r="K3">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>160.08</v>
+      </c>
+      <c r="M3">
+        <v>1810</v>
+      </c>
+      <c r="N3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>1710</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>160.08</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>1499.92</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>160.08</v>
+      </c>
+      <c r="M4">
+        <v>1710</v>
+      </c>
+      <c r="N4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>1610</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>160.08</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>1399.92</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+      <c r="L5">
+        <v>160.08</v>
+      </c>
+      <c r="M5">
+        <v>1610</v>
+      </c>
+      <c r="N5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1610</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>160.08</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1399.92</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6">
+        <v>160.08</v>
+      </c>
+      <c r="M6">
+        <v>1610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>